<commit_message>
Swap work lights to Kelcema
</commit_message>
<xml_diff>
--- a/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.9.xlsx
+++ b/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.9.xlsx
@@ -476,10 +476,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W128"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1023,7 +1023,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>7</v>
@@ -1056,7 +1056,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>7</v>
@@ -1089,7 +1089,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D20" s="4" t="n">
         <v>7</v>
@@ -1671,7 +1671,7 @@
         <v>49</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D38" s="4" t="n">
         <v>2</v>
@@ -1704,7 +1704,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D39" s="4" t="n">
         <v>2</v>
@@ -1737,7 +1737,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D40" s="4" t="n">
         <v>2</v>
@@ -4138,6 +4138,7 @@
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Add missing upstage truss run
</commit_message>
<xml_diff>
--- a/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.9.xlsx
+++ b/events/blfc/2023/BLFC 2023 Main Stage Gear List v3.9.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="93">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -112,6 +112,12 @@
     <t xml:space="preserve">Backstage &amp; Stair </t>
   </si>
   <si>
+    <t xml:space="preserve">Christie B Truss 8'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truss</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spanset 8'</t>
   </si>
   <si>
@@ -173,12 +179,6 @@
   </si>
   <si>
     <t xml:space="preserve">Work Ligts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christie B Truss 8'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truss</t>
   </si>
   <si>
     <t xml:space="preserve">Christie B Link Bar 30° </t>
@@ -476,10 +476,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W1048576"/>
+  <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1125,7 +1125,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
@@ -1152,7 +1152,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>13</v>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>13</v>
@@ -1214,10 +1214,18 @@
       <c r="W23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1238,49 +1246,41 @@
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>34</v>
-      </c>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="4" t="n">
-        <v>6</v>
-      </c>
+      <c r="E25" s="4"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="26" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4" t="n">
+        <v>6</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -1302,16 +1302,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
@@ -1335,16 +1335,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>39</v>
@@ -1401,16 +1401,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
@@ -1434,16 +1434,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>42</v>
@@ -1499,16 +1499,16 @@
       <c r="W32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="9" t="n">
+      <c r="D33" s="4" t="n">
         <v>18</v>
       </c>
       <c r="E33" s="4"/>
@@ -1532,11 +1532,11 @@
       <c r="W33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>11</v>
+      <c r="A34" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>13</v>
@@ -1565,17 +1565,17 @@
       <c r="W34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="4" t="n">
-        <v>4</v>
+      <c r="D35" s="9" t="n">
+        <v>18</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="5"/>
@@ -1599,10 +1599,10 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>13</v>
@@ -1632,10 +1632,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>13</v>
@@ -1665,16 +1665,16 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
@@ -1698,10 +1698,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>23</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
@@ -1764,16 +1764,16 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D41" s="4" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
@@ -1797,16 +1797,16 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="4" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>54</v>
@@ -1839,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="D43" s="4" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
@@ -1863,10 +1863,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>13</v>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>57</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>57</v>
@@ -2028,16 +2028,16 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
@@ -2064,7 +2064,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>13</v>
@@ -2094,10 +2094,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>13</v>
@@ -2126,10 +2126,18 @@
       <c r="W51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="A52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="4" t="n">
+        <v>6</v>
+      </c>
       <c r="E52" s="4"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -2150,16 +2158,12 @@
       <c r="V52" s="6"/>
       <c r="W52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
-        <v>60</v>
-      </c>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="E53" s="4"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
@@ -2179,49 +2183,47 @@
       <c r="V53" s="6"/>
       <c r="W53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
-      <c r="U54" s="2"/>
+    <row r="54" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D55" s="4" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2230,20 +2232,20 @@
       <c r="I55" s="4"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
       <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
+      <c r="O55" s="4"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
       <c r="U55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>61</v>
@@ -2252,7 +2254,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="4" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2274,16 +2276,16 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D57" s="4" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2305,7 +2307,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>62</v>
@@ -2314,7 +2316,7 @@
         <v>23</v>
       </c>
       <c r="D58" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2336,13 +2338,13 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>2</v>
@@ -2367,7 +2369,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>62</v>
@@ -2379,37 +2381,35 @@
         <v>2</v>
       </c>
       <c r="E60" s="4"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8"/>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8"/>
-      <c r="S60" s="8"/>
-      <c r="T60" s="8"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="6"/>
-      <c r="W60" s="6"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
+      <c r="U60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D61" s="4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="5"/>
@@ -2433,16 +2433,16 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D62" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
@@ -2466,16 +2466,16 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="4" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
@@ -2499,16 +2499,16 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D64" s="4" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="5"/>
@@ -2532,16 +2532,16 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D65" s="4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="5"/>
@@ -2564,10 +2564,18 @@
       <c r="W65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
+      <c r="A66" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="4" t="n">
+        <v>4</v>
+      </c>
       <c r="E66" s="4"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -2588,52 +2596,52 @@
       <c r="V66" s="6"/>
       <c r="W66" s="6"/>
     </row>
-    <row r="67" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="11" t="s">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="8"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="8"/>
+      <c r="Q67" s="8"/>
+      <c r="R67" s="8"/>
+      <c r="S67" s="8"/>
+      <c r="T67" s="8"/>
+      <c r="U67" s="8"/>
+      <c r="V67" s="6"/>
+      <c r="W67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="7" t="n">
+      <c r="E68" s="7" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="4" t="s">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D68" s="4" t="n">
+      <c r="C69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="8"/>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="8"/>
-      <c r="R68" s="8"/>
-      <c r="S68" s="8"/>
-      <c r="T68" s="8"/>
-      <c r="U68" s="8"/>
-      <c r="V68" s="6"/>
-      <c r="W68" s="6"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
@@ -2654,16 +2662,12 @@
       <c r="V69" s="6"/>
       <c r="W69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="4" t="n">
-        <v>3</v>
-      </c>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
@@ -2683,20 +2687,16 @@
       <c r="V70" s="6"/>
       <c r="W70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E71" s="4"/>
+    <row r="71" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
@@ -2718,16 +2718,16 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="5"/>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>73</v>
@@ -2760,7 +2760,7 @@
         <v>13</v>
       </c>
       <c r="D73" s="4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="5"/>
@@ -2784,16 +2784,16 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="4" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="5"/>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>13</v>
@@ -2850,10 +2850,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>13</v>
@@ -2883,16 +2883,16 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D77" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="5"/>
@@ -2916,16 +2916,16 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D78" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="5"/>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>31</v>
@@ -2958,7 +2958,7 @@
         <v>13</v>
       </c>
       <c r="D79" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="5"/>
@@ -2985,7 +2985,7 @@
         <v>32</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>13</v>
@@ -3015,10 +3015,10 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>13</v>
@@ -3047,10 +3047,18 @@
       <c r="W81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="A82" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="E82" s="4"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
@@ -3071,16 +3079,12 @@
       <c r="V82" s="6"/>
       <c r="W82" s="6"/>
     </row>
-    <row r="83" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
-        <v>76</v>
-      </c>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="8"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
-      <c r="E83" s="4" t="n">
-        <v>3</v>
-      </c>
+      <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -3100,43 +3104,41 @@
       <c r="V83" s="6"/>
       <c r="W83" s="6"/>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D84" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="4"/>
-      <c r="R84" s="4"/>
-      <c r="S84" s="4"/>
-      <c r="T84" s="4"/>
-      <c r="U84" s="4"/>
+    <row r="84" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="8"/>
+      <c r="Q84" s="8"/>
+      <c r="R84" s="8"/>
+      <c r="S84" s="8"/>
+      <c r="T84" s="8"/>
+      <c r="U84" s="8"/>
+      <c r="V84" s="6"/>
+      <c r="W84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>13</v>
@@ -3164,10 +3166,10 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>13</v>
@@ -3195,16 +3197,16 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D87" s="4" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -3226,16 +3228,16 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -3243,17 +3245,21 @@
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="J88" s="2"/>
-      <c r="L88" s="2"/>
-      <c r="M88" s="2"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
       <c r="N88" s="4"/>
       <c r="O88" s="4"/>
       <c r="P88" s="2"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+      <c r="U88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>78</v>
@@ -3262,7 +3268,7 @@
         <v>13</v>
       </c>
       <c r="D89" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -3280,7 +3286,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>78</v>
@@ -3307,16 +3313,16 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D91" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -3337,7 +3343,7 @@
         <v>32</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>13</v>
@@ -3361,10 +3367,10 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>13</v>
@@ -3387,10 +3393,18 @@
       <c r="S93" s="2"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
+      <c r="A94" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -3405,89 +3419,91 @@
       <c r="R94" s="2"/>
       <c r="S94" s="2"/>
     </row>
-    <row r="95" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
-        <v>80</v>
-      </c>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
       <c r="J95" s="2"/>
-      <c r="K95" s="4"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
       <c r="P95" s="2"/>
-      <c r="Q95" s="4"/>
       <c r="R95" s="2"/>
       <c r="S95" s="2"/>
-      <c r="T95" s="4"/>
-      <c r="U95" s="4"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
-        <v>81</v>
+    </row>
+    <row r="96" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B96" s="4"/>
-      <c r="C96" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D96" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="E96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
       <c r="J96" s="2"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="4"/>
-      <c r="M96" s="4"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
       <c r="N96" s="4"/>
       <c r="O96" s="4"/>
       <c r="P96" s="2"/>
       <c r="Q96" s="4"/>
-      <c r="R96" s="4"/>
-      <c r="S96" s="4"/>
+      <c r="R96" s="2"/>
+      <c r="S96" s="2"/>
       <c r="T96" s="4"/>
       <c r="U96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="s">
-        <v>82</v>
+      <c r="A97" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D97" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="2"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+      <c r="U97" s="4"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D98" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
@@ -3496,8 +3512,8 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
-        <v>67</v>
+      <c r="A99" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4" t="s">
@@ -3511,22 +3527,10 @@
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
-      <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
-      <c r="M99" s="2"/>
-      <c r="N99" s="2"/>
-      <c r="O99" s="2"/>
-      <c r="P99" s="2"/>
-      <c r="Q99" s="2"/>
-      <c r="R99" s="2"/>
-      <c r="S99" s="2"/>
-      <c r="T99" s="2"/>
-      <c r="U99" s="2"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
@@ -3555,14 +3559,14 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D101" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -3571,22 +3575,28 @@
       <c r="I101" s="4"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
-      <c r="L101" s="4"/>
+      <c r="L101" s="2"/>
       <c r="M101" s="2"/>
-      <c r="N101" s="4"/>
+      <c r="N101" s="2"/>
       <c r="O101" s="2"/>
-      <c r="P101" s="4"/>
+      <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
-      <c r="S101" s="4"/>
+      <c r="S101" s="2"/>
       <c r="T101" s="2"/>
-      <c r="U101" s="4"/>
+      <c r="U101" s="2"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2"/>
+      <c r="A102" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
+      <c r="C102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
@@ -3605,16 +3615,12 @@
       <c r="T102" s="2"/>
       <c r="U102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3" t="s">
-        <v>86</v>
-      </c>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
-      <c r="E103" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="E103" s="4"/>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
@@ -3632,42 +3638,40 @@
       <c r="T103" s="2"/>
       <c r="U103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
-        <v>87</v>
+    <row r="104" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B104" s="4"/>
-      <c r="C104" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D104" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
+      <c r="L104" s="4"/>
       <c r="M104" s="2"/>
-      <c r="N104" s="2"/>
+      <c r="N104" s="4"/>
       <c r="O104" s="2"/>
-      <c r="P104" s="2"/>
+      <c r="P104" s="4"/>
       <c r="Q104" s="2"/>
       <c r="R104" s="2"/>
-      <c r="S104" s="2"/>
+      <c r="S104" s="4"/>
       <c r="T104" s="2"/>
-      <c r="U104" s="2"/>
+      <c r="U104" s="4"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D105" s="4" t="n">
         <v>1</v>
@@ -3692,14 +3696,14 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D106" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
@@ -3721,14 +3725,14 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D107" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
@@ -3750,7 +3754,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
@@ -3778,10 +3782,16 @@
       <c r="U108" s="2"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2"/>
+      <c r="A109" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="C109" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -3800,10 +3810,8 @@
       <c r="T109" s="2"/>
       <c r="U109" s="2"/>
     </row>
-    <row r="110" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="12" t="s">
-        <v>92</v>
-      </c>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
@@ -3825,15 +3833,14 @@
       <c r="T110" s="2"/>
       <c r="U110" s="2"/>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2"/>
+    <row r="111" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
-      <c r="E111" s="4" t="n">
-        <f aca="false">SUM(E2:E104)</f>
-        <v>16</v>
-      </c>
+      <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
@@ -3856,7 +3863,10 @@
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
+      <c r="E112" s="4" t="n">
+        <f aca="false">SUM(E2:E105)</f>
+        <v>16</v>
+      </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
@@ -3911,8 +3921,8 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="2"/>
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
       <c r="R114" s="2"/>
@@ -3934,8 +3944,8 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
-      <c r="N115" s="2"/>
-      <c r="O115" s="2"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
       <c r="R115" s="2"/>
@@ -3978,18 +3988,18 @@
       <c r="I117" s="4"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
-      <c r="L117" s="4"/>
-      <c r="M117" s="4"/>
-      <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
       <c r="R117" s="2"/>
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
     </row>
-    <row r="118" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -4001,18 +4011,19 @@
       <c r="I118" s="4"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
-      <c r="L118" s="2"/>
-      <c r="M118" s="2"/>
-      <c r="N118" s="2"/>
-      <c r="O118" s="2"/>
-      <c r="P118" s="2"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
       <c r="Q118" s="2"/>
       <c r="R118" s="2"/>
       <c r="S118" s="2"/>
       <c r="T118" s="2"/>
       <c r="U118" s="2"/>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
@@ -4032,6 +4043,7 @@
       <c r="R119" s="2"/>
       <c r="S119" s="2"/>
       <c r="T119" s="2"/>
+      <c r="U119" s="2"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="4"/>
@@ -4083,6 +4095,18 @@
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+      <c r="N122" s="2"/>
+      <c r="O122" s="2"/>
+      <c r="P122" s="2"/>
+      <c r="Q122" s="2"/>
+      <c r="R122" s="2"/>
+      <c r="S122" s="2"/>
+      <c r="T122" s="2"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="4"/>
@@ -4138,7 +4162,15 @@
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>